<commit_message>
Corrección de código de una imagen
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion01/SolicitudGrafica_CN_09_01_CO_REC10.xlsx
+++ b/fuentes/contenidos/grado09/guion01/SolicitudGrafica_CN_09_01_CO_REC10.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\Desktop\Procesar Magda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado09\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="hX79YNGfHMUCcosWMoH0GQuhNo2gkebFrfW3do2TOcvwqaujU9m0uwOL5UkRtWEspAy/ISD2JB8+jf057W9mVA==" workbookSaltValue="uRz/CDpmZ5ecKheoN1C0Jw==" workbookSpinCount="100000" lockStructure="1"/>
@@ -2542,8 +2542,8 @@
   <dimension ref="A1:P108"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <pane ySplit="9" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3240,7 +3240,7 @@
         <v>IMG10</v>
       </c>
       <c r="B19" s="62">
-        <v>128300303</v>
+        <v>93030028</v>
       </c>
       <c r="C19" s="20" t="str">
         <f t="shared" si="0"/>

</xml_diff>